<commit_message>
Changes on Portfolio page.
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Incubator\Studying\Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2A1AF8-7388-40CB-A8D8-78DA97CB683E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D931417-48B6-4C41-9551-73E00F2CA0BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="37470" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>HTML &amp; CSS</t>
   </si>
@@ -100,13 +100,25 @@
   </si>
   <si>
     <t>skill: '</t>
+  </si>
+  <si>
+    <t>link: '</t>
+  </si>
+  <si>
+    <t>https://tonyfinder.github.io/Pedicure_Goods/</t>
+  </si>
+  <si>
+    <t>https://tonyfinder.github.io/React-Samurai/</t>
+  </si>
+  <si>
+    <t>https://tonyfinder.github.io/Todolist/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +145,14 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -148,7 +168,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -229,11 +249,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -251,8 +309,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -531,28 +600,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21:J31"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21:K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="71.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="107.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="74.85546875" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="6" max="6" width="133.42578125" customWidth="1"/>
+    <col min="7" max="7" width="74.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -563,7 +633,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -573,20 +643,20 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="str">
+      <c r="F3" t="str">
         <f>CONCATENATE("{",$A$2,A3,", ",$B$2,B3,"', ",$C$2,C3,"'},")</f>
         <v>{id: 1, skill: 'HTML &amp; CSS', description: 'Like to use flex methods.'},</v>
       </c>
-      <c r="F3" s="3" t="str">
-        <f>CONCATENATE("skills: [",E3,E4,E5,E6,E7,"],")</f>
+      <c r="G3" s="3" t="str">
+        <f>CONCATENATE("skills: [",F3,F4,F5,F6,F7,"],")</f>
         <v>skills: [{id: 1, skill: 'HTML &amp; CSS', description: 'Like to use flex methods.'},{id: 2, skill: 'JavaScript', description: 'Good programming language… but TypeScript is just the best!'},{id: 3, skill: 'TypeScript', description: 'This is the best programming language to know. I have a very good skills here.'},{id: 4, skill: 'React', description: 'I am focused here. So here is my way!'},{id: 5, skill: 'Redux', description: 'If you see this portfolio, it means that I already have good knowledge here.'},],</v>
       </c>
-      <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -596,17 +666,17 @@
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="str">
-        <f t="shared" ref="E4:E7" si="0">CONCATENATE("{",$A$2,A4,", ",$B$2,B4,"', ",$C$2,C4,"'},")</f>
+      <c r="F4" t="str">
+        <f t="shared" ref="F4:F7" si="0">CONCATENATE("{",$A$2,A4,", ",$B$2,B4,"', ",$C$2,C4,"'},")</f>
         <v>{id: 2, skill: 'JavaScript', description: 'Good programming language… but TypeScript is just the best!'},</v>
       </c>
-      <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -616,17 +686,17 @@
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E5" t="str">
+      <c r="F5" t="str">
         <f t="shared" si="0"/>
         <v>{id: 3, skill: 'TypeScript', description: 'This is the best programming language to know. I have a very good skills here.'},</v>
       </c>
-      <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -636,17 +706,17 @@
       <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E6" t="str">
+      <c r="F6" t="str">
         <f t="shared" si="0"/>
         <v>{id: 4, skill: 'React', description: 'I am focused here. So here is my way!'},</v>
       </c>
-      <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -656,25 +726,26 @@
       <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E7" t="str">
+      <c r="F7" t="str">
         <f t="shared" si="0"/>
         <v>{id: 5, skill: 'Redux', description: 'If you see this portfolio, it means that I already have good knowledge here.'},</v>
       </c>
-      <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="K7" s="3"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -684,8 +755,11 @@
       <c r="C12" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D12" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -695,20 +769,23 @@
       <c r="C13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E13" t="str">
-        <f>CONCATENATE("{",$A$12,A13,", ",$B$12,B13,"', ",$C$12,C13,"'},")</f>
-        <v>{id: 1, name: 'To Do list', description: 'The main project I have been made using TypeScript and React'},</v>
-      </c>
-      <c r="F13" s="3" t="str">
-        <f>CONCATENATE("portfolio: [",E13,E14,E15,"],")</f>
-        <v>portfolio: [{id: 1, name: 'To Do list', description: 'The main project I have been made using TypeScript and React'},{id: 2, name: 'Social network', description: 'Introducing of my code using TypeScript and React'},{id: 3, name: 'Pedicure goods', description: 'This app was made for personal use only'},],</v>
-      </c>
-      <c r="G13" s="3"/>
+      <c r="D13" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" t="str">
+        <f>CONCATENATE("{",$A$12,A13,", ",$B$12,B13,"', ",$C$12,C13,"', ",$D$12,D13,"'},")</f>
+        <v>{id: 1, name: 'To Do list', description: 'The main project I have been made using TypeScript and React', link: 'https://tonyfinder.github.io/Todolist/'},</v>
+      </c>
+      <c r="G13" s="3" t="str">
+        <f>CONCATENATE("portfolio: [",F13,F14,F15,"],")</f>
+        <v>portfolio: [{id: 1, name: 'To Do list', description: 'The main project I have been made using TypeScript and React', link: 'https://tonyfinder.github.io/Todolist/'},{id: 2, name: 'Social network', description: 'Introducing of my code using TypeScript and React', link: 'https://tonyfinder.github.io/React-Samurai/'},{id: 3, name: 'Pedicure goods', description: 'This app was made for personal use only', link: 'https://tonyfinder.github.io/Pedicure_Goods/'},],</v>
+      </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -718,17 +795,20 @@
       <c r="C14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E14" t="str">
-        <f t="shared" ref="E14:E15" si="1">CONCATENATE("{",$A$12,A14,", ",$B$12,B14,"', ",$C$12,C14,"'},")</f>
-        <v>{id: 2, name: 'Social network', description: 'Introducing of my code using TypeScript and React'},</v>
-      </c>
-      <c r="F14" s="3"/>
+      <c r="D14" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" ref="F14:F15" si="1">CONCATENATE("{",$A$12,A14,", ",$B$12,B14,"', ",$C$12,C14,"', ",$D$12,D14,"'},")</f>
+        <v>{id: 2, name: 'Social network', description: 'Introducing of my code using TypeScript and React', link: 'https://tonyfinder.github.io/React-Samurai/'},</v>
+      </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>3</v>
       </c>
@@ -738,119 +818,127 @@
       <c r="C15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E15" t="str">
+      <c r="D15" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 3, name: 'Pedicure goods', description: 'This app was made for personal use only'},</v>
-      </c>
-      <c r="F15" s="3"/>
+        <v>{id: 3, name: 'Pedicure goods', description: 'This app was made for personal use only', link: 'https://tonyfinder.github.io/Pedicure_Goods/'},</v>
+      </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F16" s="3"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
-    </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F17" s="3"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
-    </row>
-    <row r="21" spans="6:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F21" s="3" t="str">
-        <f>CONCATENATE("{",F3," ",F13,"}")</f>
-        <v>{skills: [{id: 1, skill: 'HTML &amp; CSS', description: 'Like to use flex methods.'},{id: 2, skill: 'JavaScript', description: 'Good programming language… but TypeScript is just the best!'},{id: 3, skill: 'TypeScript', description: 'This is the best programming language to know. I have a very good skills here.'},{id: 4, skill: 'React', description: 'I am focused here. So here is my way!'},{id: 5, skill: 'Redux', description: 'If you see this portfolio, it means that I already have good knowledge here.'},], portfolio: [{id: 1, name: 'To Do list', description: 'The main project I have been made using TypeScript and React'},{id: 2, name: 'Social network', description: 'Introducing of my code using TypeScript and React'},{id: 3, name: 'Pedicure goods', description: 'This app was made for personal use only'},],}</v>
-      </c>
-      <c r="G21" s="3"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="21" spans="7:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="3" t="str">
+        <f>CONCATENATE("{",G3," ",G13,"}")</f>
+        <v>{skills: [{id: 1, skill: 'HTML &amp; CSS', description: 'Like to use flex methods.'},{id: 2, skill: 'JavaScript', description: 'Good programming language… but TypeScript is just the best!'},{id: 3, skill: 'TypeScript', description: 'This is the best programming language to know. I have a very good skills here.'},{id: 4, skill: 'React', description: 'I am focused here. So here is my way!'},{id: 5, skill: 'Redux', description: 'If you see this portfolio, it means that I already have good knowledge here.'},], portfolio: [{id: 1, name: 'To Do list', description: 'The main project I have been made using TypeScript and React', link: 'https://tonyfinder.github.io/Todolist/'},{id: 2, name: 'Social network', description: 'Introducing of my code using TypeScript and React', link: 'https://tonyfinder.github.io/React-Samurai/'},{id: 3, name: 'Pedicure goods', description: 'This app was made for personal use only', link: 'https://tonyfinder.github.io/Pedicure_Goods/'},],}</v>
+      </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
-    </row>
-    <row r="22" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F22" s="3"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F23" s="3"/>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F24" s="3"/>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
-    </row>
-    <row r="25" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F25" s="3"/>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
-    </row>
-    <row r="26" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F26" s="3"/>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
-    </row>
-    <row r="27" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F27" s="3"/>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
-    </row>
-    <row r="28" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F28" s="3"/>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
-    </row>
-    <row r="29" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F29" s="3"/>
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
-    </row>
-    <row r="30" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F30" s="3"/>
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
-    </row>
-    <row r="31" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F31" s="3"/>
+      <c r="K30" s="3"/>
+    </row>
+    <row r="31" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="F3:J7"/>
+    <mergeCell ref="G3:K7"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="F13:J17"/>
-    <mergeCell ref="F21:J31"/>
+    <mergeCell ref="G13:K17"/>
+    <mergeCell ref="G21:K31"/>
+    <mergeCell ref="A11:D11"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D15" r:id="rId1" xr:uid="{60D261D6-A2F0-4FB0-8231-FCFB8CBA8308}"/>
+    <hyperlink ref="D14" r:id="rId2" xr:uid="{B55D9F06-F9AF-4BAA-AC54-787CA4AF6350}"/>
+    <hyperlink ref="D13" r:id="rId3" xr:uid="{A5F18E14-298A-436F-BAAD-4E22AE5B81CD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added all the rest pages + @media.
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Incubator\Studying\Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D931417-48B6-4C41-9551-73E00F2CA0BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02A1258-D375-449A-8BD6-E2774E39696B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="-120" windowWidth="37470" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,9 +78,6 @@
     <t>Portfolio</t>
   </si>
   <si>
-    <t>To Do list</t>
-  </si>
-  <si>
     <t>Social network</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>https://tonyfinder.github.io/Todolist/</t>
+  </si>
+  <si>
+    <t>To-do list</t>
   </si>
 </sst>
 </file>
@@ -297,6 +297,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -318,7 +319,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -602,38 +602,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21:K31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="71.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" customWidth="1"/>
-    <col min="6" max="6" width="133.42578125" customWidth="1"/>
-    <col min="7" max="7" width="74.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1"/>
+    <col min="6" max="6" width="133.44140625" customWidth="1"/>
+    <col min="7" max="7" width="74.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="6"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -647,16 +647,16 @@
         <f>CONCATENATE("{",$A$2,A3,", ",$B$2,B3,"', ",$C$2,C3,"'},")</f>
         <v>{id: 1, skill: 'HTML &amp; CSS', description: 'Like to use flex methods.'},</v>
       </c>
-      <c r="G3" s="3" t="str">
+      <c r="G3" s="4" t="str">
         <f>CONCATENATE("skills: [",F3,F4,F5,F6,F7,"],")</f>
         <v>skills: [{id: 1, skill: 'HTML &amp; CSS', description: 'Like to use flex methods.'},{id: 2, skill: 'JavaScript', description: 'Good programming language… but TypeScript is just the best!'},{id: 3, skill: 'TypeScript', description: 'This is the best programming language to know. I have a very good skills here.'},{id: 4, skill: 'React', description: 'I am focused here. So here is my way!'},{id: 5, skill: 'Redux', description: 'If you see this portfolio, it means that I already have good knowledge here.'},],</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -670,13 +670,13 @@
         <f t="shared" ref="F4:F7" si="0">CONCATENATE("{",$A$2,A4,", ",$B$2,B4,"', ",$C$2,C4,"'},")</f>
         <v>{id: 2, skill: 'JavaScript', description: 'Good programming language… but TypeScript is just the best!'},</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -690,13 +690,13 @@
         <f t="shared" si="0"/>
         <v>{id: 3, skill: 'TypeScript', description: 'This is the best programming language to know. I have a very good skills here.'},</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -704,19 +704,19 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
         <v>{id: 4, skill: 'React', description: 'I am focused here. So here is my way!'},</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -730,22 +730,22 @@
         <f t="shared" si="0"/>
         <v>{id: 5, skill: 'Redux', description: 'If you see this portfolio, it means that I already have good knowledge here.'},</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="10"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -756,174 +756,174 @@
         <v>11</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="F13" t="str">
         <f>CONCATENATE("{",$A$12,A13,", ",$B$12,B13,"', ",$C$12,C13,"', ",$D$12,D13,"'},")</f>
-        <v>{id: 1, name: 'To Do list', description: 'The main project I have been made using TypeScript and React', link: 'https://tonyfinder.github.io/Todolist/'},</v>
-      </c>
-      <c r="G13" s="3" t="str">
+        <v>{id: 1, name: 'To-do list', description: 'The main project I have been made using TypeScript and React', link: 'https://tonyfinder.github.io/Todolist/'},</v>
+      </c>
+      <c r="G13" s="4" t="str">
         <f>CONCATENATE("portfolio: [",F13,F14,F15,"],")</f>
-        <v>portfolio: [{id: 1, name: 'To Do list', description: 'The main project I have been made using TypeScript and React', link: 'https://tonyfinder.github.io/Todolist/'},{id: 2, name: 'Social network', description: 'Introducing of my code using TypeScript and React', link: 'https://tonyfinder.github.io/React-Samurai/'},{id: 3, name: 'Pedicure goods', description: 'This app was made for personal use only', link: 'https://tonyfinder.github.io/Pedicure_Goods/'},],</v>
-      </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>portfolio: [{id: 1, name: 'To-do list', description: 'The main project I have been made using TypeScript and React', link: 'https://tonyfinder.github.io/Todolist/'},{id: 2, name: 'Social network', description: 'Introducing of my code using TypeScript and React', link: 'https://tonyfinder.github.io/React-Samurai/'},{id: 3, name: 'Pedicure goods', description: 'This app was made for personal use only', link: 'https://tonyfinder.github.io/Pedicure_Goods/'},],</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>24</v>
+        <v>16</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" ref="F14:F15" si="1">CONCATENATE("{",$A$12,A14,", ",$B$12,B14,"', ",$C$12,C14,"', ",$D$12,D14,"'},")</f>
         <v>{id: 2, name: 'Social network', description: 'Introducing of my code using TypeScript and React', link: 'https://tonyfinder.github.io/React-Samurai/'},</v>
       </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>23</v>
+        <v>17</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="1"/>
         <v>{id: 3, name: 'Pedicure goods', description: 'This app was made for personal use only', link: 'https://tonyfinder.github.io/Pedicure_Goods/'},</v>
       </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-    </row>
-    <row r="21" spans="7:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G21" s="3" t="str">
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="21" spans="7:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G21" s="4" t="str">
         <f>CONCATENATE("{",G3," ",G13,"}")</f>
-        <v>{skills: [{id: 1, skill: 'HTML &amp; CSS', description: 'Like to use flex methods.'},{id: 2, skill: 'JavaScript', description: 'Good programming language… but TypeScript is just the best!'},{id: 3, skill: 'TypeScript', description: 'This is the best programming language to know. I have a very good skills here.'},{id: 4, skill: 'React', description: 'I am focused here. So here is my way!'},{id: 5, skill: 'Redux', description: 'If you see this portfolio, it means that I already have good knowledge here.'},], portfolio: [{id: 1, name: 'To Do list', description: 'The main project I have been made using TypeScript and React', link: 'https://tonyfinder.github.io/Todolist/'},{id: 2, name: 'Social network', description: 'Introducing of my code using TypeScript and React', link: 'https://tonyfinder.github.io/React-Samurai/'},{id: 3, name: 'Pedicure goods', description: 'This app was made for personal use only', link: 'https://tonyfinder.github.io/Pedicure_Goods/'},],}</v>
-      </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-    </row>
-    <row r="22" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-    </row>
-    <row r="23" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-    </row>
-    <row r="24" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-    </row>
-    <row r="25" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-    </row>
-    <row r="26" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-    </row>
-    <row r="27" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-    </row>
-    <row r="28" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-    </row>
-    <row r="29" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-    </row>
-    <row r="30" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-    </row>
-    <row r="31" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
+        <v>{skills: [{id: 1, skill: 'HTML &amp; CSS', description: 'Like to use flex methods.'},{id: 2, skill: 'JavaScript', description: 'Good programming language… but TypeScript is just the best!'},{id: 3, skill: 'TypeScript', description: 'This is the best programming language to know. I have a very good skills here.'},{id: 4, skill: 'React', description: 'I am focused here. So here is my way!'},{id: 5, skill: 'Redux', description: 'If you see this portfolio, it means that I already have good knowledge here.'},], portfolio: [{id: 1, name: 'To-do list', description: 'The main project I have been made using TypeScript and React', link: 'https://tonyfinder.github.io/Todolist/'},{id: 2, name: 'Social network', description: 'Introducing of my code using TypeScript and React', link: 'https://tonyfinder.github.io/React-Samurai/'},{id: 3, name: 'Pedicure goods', description: 'This app was made for personal use only', link: 'https://tonyfinder.github.io/Pedicure_Goods/'},],}</v>
+      </c>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+    </row>
+    <row r="22" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+    </row>
+    <row r="24" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+    </row>
+    <row r="25" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+    </row>
+    <row r="26" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+    </row>
+    <row r="27" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+    </row>
+    <row r="28" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+    </row>
+    <row r="29" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+    </row>
+    <row r="30" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+    </row>
+    <row r="31" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>